<commit_message>
Passage du xlsx au json
</commit_message>
<xml_diff>
--- a/models/analyse_clusters.xlsx
+++ b/models/analyse_clusters.xlsx
@@ -470,19 +470,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19992.5</v>
+        <v>19950</v>
       </c>
       <c r="C2" t="n">
-        <v>112225</v>
+        <v>79985</v>
       </c>
       <c r="D2" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="E2" t="n">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F2" t="n">
-        <v>732</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>24490</v>
+        <v>11775</v>
       </c>
       <c r="C3" t="n">
-        <v>52870</v>
+        <v>82698</v>
       </c>
       <c r="D3" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E3" t="n">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="F3" t="n">
-        <v>799</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20825</v>
+        <v>23885</v>
       </c>
       <c r="C4" t="n">
-        <v>75380.5</v>
+        <v>68783.5</v>
       </c>
       <c r="D4" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E4" t="n">
-        <v>113.5</v>
+        <v>125</v>
       </c>
       <c r="F4" t="n">
-        <v>154</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>11990</v>
+        <v>32990</v>
       </c>
       <c r="C5" t="n">
-        <v>70954</v>
+        <v>58000</v>
       </c>
       <c r="D5" t="n">
         <v>2017</v>
       </c>
       <c r="E5" t="n">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="F5" t="n">
-        <v>547</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>22780</v>
+        <v>13990</v>
       </c>
       <c r="C6" t="n">
-        <v>43690</v>
+        <v>89000</v>
       </c>
       <c r="D6" t="n">
-        <v>2020</v>
+        <v>2016.5</v>
       </c>
       <c r="E6" t="n">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="F6" t="n">
-        <v>417</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>